<commit_message>
memperbaiki bug: navigasi hasil selalu ke hasil-1
</commit_message>
<xml_diff>
--- a/tmp/Book2.xlsx
+++ b/tmp/Book2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\belajar-phpspreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F06AD7CF-8CBF-4728-A600-EB9DFF11C564}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E28EF7A-F1D4-46F0-9693-F7D4DEB73D64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A8709DDE-C6C4-4EA5-A471-400F8EBF0FAA}"/>
   </bookViews>
@@ -55,8 +55,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
-    <font>
+  <fonts count="8" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -146,38 +154,41 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -496,39 +507,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65E5783-8773-4266-9D0A-473E85629102}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+    </row>
+    <row r="2" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>